<commit_message>
Funciona para cualquier computador
</commit_message>
<xml_diff>
--- a/DatosPrueba.xlsx
+++ b/DatosPrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joaquin\Desktop\Constituyente\trabajoconstituyente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A91B9-CF99-40D9-9E8A-2F99D912744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8CE2CF-AB6E-405D-9BF8-BBE954169298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="405" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -910,16 +910,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1094,7 +1091,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1116,7 +1113,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1127,7 +1124,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1138,7 +1135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1160,7 +1157,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1182,7 +1179,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1193,7 +1190,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1204,7 +1201,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1215,7 +1212,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1226,7 +1223,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1237,7 +1234,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1247,9 +1244,8 @@
       <c r="C30" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1260,7 +1256,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1388,6 +1384,7 @@
       <c r="B43" t="s">
         <v>43</v>
       </c>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">

</xml_diff>

<commit_message>
modelo fusionado con interfaz funcionando
</commit_message>
<xml_diff>
--- a/DatosPrueba.xlsx
+++ b/DatosPrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joaquin\Desktop\Constituyente\trabajoconstituyente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8CE2CF-AB6E-405D-9BF8-BBE954169298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22C1CC6-C7F6-4D38-A00A-A53EC928103B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="405" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,14 +516,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -566,12 +558,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -1384,7 +1375,6 @@
       <c r="B43" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -2622,6 +2612,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>